<commit_message>
ajout la logique de tick
</commit_message>
<xml_diff>
--- a/src/reports/trades_history.xlsx
+++ b/src/reports/trades_history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -653,6 +653,465 @@
         <v>0.6260995833333334</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>103764.81</v>
+      </c>
+      <c r="C5" t="n">
+        <v>103866.18</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1013699999999953</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1013699999999953</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.09769207884637897</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>02:10:02</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>02:12:33</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>2.52413535</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>103878.15</v>
+      </c>
+      <c r="C6" t="n">
+        <v>103935.21121</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.05706120999999985</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.05706120999999985</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.05493090702905264</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>02:12:39</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>02:15:30</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>2.849939516666667</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>103854.94</v>
+      </c>
+      <c r="C7" t="n">
+        <v>103918.67704</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.06373703999999271</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.06373703999999271</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.06137121642937033</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>02:16:31</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>02:17:42</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>1.191119316666666</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>103832.73</v>
+      </c>
+      <c r="C8" t="n">
+        <v>103949.8474</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.1171174000000028</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1171174000000028</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.1127942990615799</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>02:31:38</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>02:32:47</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>1.157217583333333</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>103909.64137</v>
+      </c>
+      <c r="C9" t="n">
+        <v>103974.21</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.06456863000000886</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.06456863000000886</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.06213920974868326</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>06:42:39</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>07:06:21</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>23.70910848333333</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>103916.61</v>
+      </c>
+      <c r="C10" t="n">
+        <v>103971.42417</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.05481416999999783</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.05481416999999783</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.05274822764137305</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>09:04:05</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>09:05:42</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>1.61504025</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>103886.27174</v>
+      </c>
+      <c r="C11" t="n">
+        <v>103500</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.3862717399999965</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-0.3862717399999965</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-0.3718217369150883</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>09:45:41</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>10:15:26</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>29.75130018333333</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>103369.35434</v>
+      </c>
+      <c r="C12" t="n">
+        <v>103431.35</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0619956600000005</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0619956600000005</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.05997489332871894</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>10:45:15</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>10:54:10</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>8.914118349999999</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>103556.4664</v>
+      </c>
+      <c r="C13" t="n">
+        <v>103615.03574</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.05856934000000183</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.05856934000000183</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.05655787806989311</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>15:01:26</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>15:06:01</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>4.578442166666666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
trois tick ( ancien commit = 2 tick
</commit_message>
<xml_diff>
--- a/src/reports/trades_history.xlsx
+++ b/src/reports/trades_history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1112,6 +1112,159 @@
         <v>4.578442166666666</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>103492.02516</v>
+      </c>
+      <c r="C14" t="n">
+        <v>103550.78</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.05875483999999415</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.05875483999999415</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.05677233575162764</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>00:49:27</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>01:00:00</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>10.55609733333333</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>103425.83464</v>
+      </c>
+      <c r="C15" t="n">
+        <v>102826.53584</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-0.5992988000000041</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-0.5992988000000041</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-0.5794478740113788</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>02:26:39</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>03:20:26</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>53.77595986666667</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>102974.83922</v>
+      </c>
+      <c r="C16" t="n">
+        <v>103081.5932</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.1067539800000086</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.1067539800000086</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.1036699652154199</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>03:29:18</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>04:25:04</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>55.75855795</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
suppression stoch et dmi/ ajout william et fisher, ajout de systeme de scoring
</commit_message>
<xml_diff>
--- a/src/reports/trades_history.xlsx
+++ b/src/reports/trades_history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1520,6 +1520,261 @@
         <v>26.99185</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>105735.23022</v>
+      </c>
+      <c r="C22" t="n">
+        <v>105969.92458</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.2346943600000086</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.2346943600000086</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.2219642020088171</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>05:54:17</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>06:50:02</t>
+        </is>
+      </c>
+      <c r="M22" t="n">
+        <v>55.74122256666667</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>105524.99</v>
+      </c>
+      <c r="C23" t="n">
+        <v>105606.17</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.08117999999999302</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.08117999999999302</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.07692964481682776</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>08:38:18</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>09:09:47</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>31.47902798333333</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>105154.25</v>
+      </c>
+      <c r="C24" t="n">
+        <v>105283.11</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.1288600000000006</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.1288600000000006</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.1225437868654862</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>09:57:18</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>11:20:02</t>
+        </is>
+      </c>
+      <c r="M24" t="n">
+        <v>82.73491846666667</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>105147.75132</v>
+      </c>
+      <c r="C25" t="n">
+        <v>105250.02</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.1022686800000083</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.1022686800000083</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.09726188027432969</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>12:44:17</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>13:36:02</t>
+        </is>
+      </c>
+      <c r="M25" t="n">
+        <v>51.74237011666666</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>110727.71075</v>
+      </c>
+      <c r="C26" t="n">
+        <v>110750.2824</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.02257164999999805</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.02257164999999805</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.02038482494319792</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>2025-05-23</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>06:46:09</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>2025-05-23</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>07:30:22</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
+        <v>44.20664878333334</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
suppression obv, remplacer dmi negatif pour valider position
</commit_message>
<xml_diff>
--- a/src/reports/trades_history.xlsx
+++ b/src/reports/trades_history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1928,6 +1928,465 @@
         <v>1.0762834</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>110073.37</v>
+      </c>
+      <c r="C30" t="n">
+        <v>110264.14734</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.1907773400000005</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.1907773400000005</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.1733183421203517</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>02:16:38</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>02:26:57</t>
+        </is>
+      </c>
+      <c r="M30" t="n">
+        <v>10.3220522</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>109850.71</v>
+      </c>
+      <c r="C31" t="n">
+        <v>109576.95</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-0.2737600000000093</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>-0.2737600000000093</v>
+      </c>
+      <c r="H31" t="n">
+        <v>-0.2492109518454722</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>03:57:39</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>04:05:57</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
+        <v>8.303035916666667</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>109606.78947</v>
+      </c>
+      <c r="C32" t="n">
+        <v>109675.18</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.06839052999998967</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.06839052999998967</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.06239625330756408</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>04:14:39</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>04:27:18</t>
+        </is>
+      </c>
+      <c r="M32" t="n">
+        <v>12.6649506</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>109538.4191</v>
+      </c>
+      <c r="C33" t="n">
+        <v>109623.4</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.08498089999999502</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.08498089999999502</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.07758090786613792</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>05:20:39</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>06:02:48</t>
+        </is>
+      </c>
+      <c r="M33" t="n">
+        <v>42.15393601666666</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>109421.77</v>
+      </c>
+      <c r="C34" t="n">
+        <v>109566.47677</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.1447067699999898</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.1447067699999898</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.1322467823359006</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>07:41:39</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>08:36:48</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
+        <v>55.14536743333333</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>109461.97</v>
+      </c>
+      <c r="C35" t="n">
+        <v>109223.09799</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-0.2388720100000064</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>-0.2388720100000064</v>
+      </c>
+      <c r="H35" t="n">
+        <v>-0.2182237447398457</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>09:13:38</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>09:37:38</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
+        <v>23.99959545</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>109211.47936</v>
+      </c>
+      <c r="C36" t="n">
+        <v>109399.35</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.1878706400000083</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.1878706400000083</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.1720246269906478</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>11:07:38</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>11:26:08</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>18.49002208333333</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>109408.938</v>
+      </c>
+      <c r="C37" t="n">
+        <v>109499.7018</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.09076380000000063</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.09076380000000063</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.08295830455826254</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>13:10:16</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>13:12:15</t>
+        </is>
+      </c>
+      <c r="M37" t="n">
+        <v>1.973762133333334</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>BTC/USDC</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>109749.57</v>
+      </c>
+      <c r="C38" t="n">
+        <v>109450.04</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-0.2995300000000134</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>-0.2995300000000134</v>
+      </c>
+      <c r="H38" t="n">
+        <v>-0.2729213426531087</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>15:27:51</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>15:35:08</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
+        <v>7.29405835</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>